<commit_message>
Preparations made for BoardGUI programming
</commit_message>
<xml_diff>
--- a/TCJPClueLayout.xlsx
+++ b/TCJPClueLayout.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\CSCI306\ClueGameTCJP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\CSCI306\ClueGameJPIT\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="606" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="606" uniqueCount="39">
   <si>
     <t>w</t>
   </si>
@@ -114,6 +114,33 @@
   </si>
   <si>
     <t>Number of doors: 16</t>
+  </si>
+  <si>
+    <t>KN</t>
+  </si>
+  <si>
+    <t>GN</t>
+  </si>
+  <si>
+    <t>RN</t>
+  </si>
+  <si>
+    <t>YN</t>
+  </si>
+  <si>
+    <t>LN</t>
+  </si>
+  <si>
+    <t>ON</t>
+  </si>
+  <si>
+    <t>BN</t>
+  </si>
+  <si>
+    <t>PN</t>
+  </si>
+  <si>
+    <t>SN</t>
   </si>
 </sst>
 </file>
@@ -513,7 +540,7 @@
   <dimension ref="A1:Y34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R14" sqref="R14"/>
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -678,7 +705,7 @@
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>4</v>
+        <v>31</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>4</v>
@@ -696,7 +723,7 @@
         <v>23</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>3</v>
+        <v>32</v>
       </c>
       <c r="H3" s="4" t="s">
         <v>3</v>
@@ -717,7 +744,7 @@
         <v>20</v>
       </c>
       <c r="N3" s="4" t="s">
-        <v>9</v>
+        <v>33</v>
       </c>
       <c r="O3" s="4" t="s">
         <v>9</v>
@@ -894,7 +921,7 @@
         <v>0</v>
       </c>
       <c r="U5" s="4" t="s">
-        <v>8</v>
+        <v>34</v>
       </c>
       <c r="V5" s="4" t="s">
         <v>8</v>
@@ -1458,7 +1485,7 @@
     </row>
     <row r="13" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>5</v>
@@ -1908,7 +1935,7 @@
         <v>10</v>
       </c>
       <c r="U18" s="4" t="s">
-        <v>10</v>
+        <v>35</v>
       </c>
       <c r="V18" s="4" t="s">
         <v>10</v>
@@ -2160,7 +2187,7 @@
     </row>
     <row r="22" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
-        <v>6</v>
+        <v>38</v>
       </c>
       <c r="B22" s="4" t="s">
         <v>6</v>
@@ -2196,7 +2223,7 @@
         <v>7</v>
       </c>
       <c r="M22" s="4" t="s">
-        <v>7</v>
+        <v>36</v>
       </c>
       <c r="N22" s="4" t="s">
         <v>7</v>
@@ -2256,7 +2283,7 @@
         <v>2</v>
       </c>
       <c r="G23" s="4" t="s">
-        <v>2</v>
+        <v>37</v>
       </c>
       <c r="H23" s="4" t="s">
         <v>2</v>

</xml_diff>